<commit_message>
adjusted power score and plotting.
</commit_message>
<xml_diff>
--- a/Datasets/comic_dataset_1.xlsx
+++ b/Datasets/comic_dataset_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noell\PycharmProjects\superheroes\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AF7502-4FC0-4DFD-9095-A14907FB7AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D0CD4F-9265-462D-BA89-C1C15FB148F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="166">
   <si>
     <t>Property</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>Power_Score</t>
+  </si>
+  <si>
+    <t>Semi</t>
   </si>
 </sst>
 </file>
@@ -877,8 +880,8 @@
   <dimension ref="A1:T121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T1" sqref="F1:T1"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,7 +1043,7 @@
         <v>134</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="G3" t="s">
         <v>133</v>
@@ -4285,7 +4288,7 @@
         <v>128</v>
       </c>
       <c r="F58" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="G58" t="s">
         <v>132</v>
@@ -6173,7 +6176,7 @@
         <v>127</v>
       </c>
       <c r="F90" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="G90" t="s">
         <v>132</v>
@@ -6586,7 +6589,7 @@
         <v>137</v>
       </c>
       <c r="F97" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="G97" t="s">
         <v>132</v>
@@ -6645,7 +6648,7 @@
         <v>128</v>
       </c>
       <c r="F98" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="G98" t="s">
         <v>132</v>
@@ -7176,7 +7179,7 @@
         <v>128</v>
       </c>
       <c r="F107" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="G107" t="s">
         <v>132</v>

</xml_diff>